<commit_message>
Bug fixes, see CHANGES.txt
</commit_message>
<xml_diff>
--- a/Example/Sampling scheme/Samples.xlsx
+++ b/Example/Sampling scheme/Samples.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="16">
   <si>
     <t>int climate</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>brick dimension</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
   <si>
     <t>Oostende</t>
@@ -452,61 +458,61 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>0.7250000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>6.25</v>
+        <v>4.5</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2">
-        <v>1.125</v>
+        <v>0.5625</v>
       </c>
       <c r="H2">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="I2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J2">
-        <v>0.4562499999999999</v>
+        <v>0.2375</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>0.75</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>4.5</v>
+        <v>1.875</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3">
-        <v>1.171875</v>
+        <v>0.65625</v>
       </c>
       <c r="H3">
-        <v>135</v>
+        <v>315</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0.325</v>
@@ -516,215 +522,215 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>0.55</v>
+        <v>0.75</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>2.75</v>
+        <v>3.625</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>0.84375</v>
       </c>
       <c r="H4">
-        <v>247.5</v>
+        <v>90</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J4">
-        <v>0.19375</v>
+        <v>0.346875</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>0.65</v>
+        <v>0.475</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>7.5625</v>
+        <v>2.75</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>0.375</v>
+        <v>1.03125</v>
       </c>
       <c r="H5">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J5">
-        <v>0.4125</v>
+        <v>0.171875</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>0.5750000000000001</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>7.125</v>
+        <v>5.375</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6">
-        <v>0.5625</v>
+        <v>0.46875</v>
       </c>
       <c r="H6">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="I6">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>0.2375</v>
+        <v>0.434375</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>2</v>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>0.7375</v>
+        <v>0.5</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>6.90625</v>
+        <v>2.3125</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>0.65625</v>
+        <v>0.1875</v>
       </c>
       <c r="H7">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="I7">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>0.36875</v>
+        <v>0.478125</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>2</v>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>0.675</v>
+        <v>0.55</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E8">
         <v>3.1875</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G8">
-        <v>1.03125</v>
+        <v>0.375</v>
       </c>
       <c r="H8">
-        <v>90</v>
+        <v>247.5</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J8">
-        <v>0.303125</v>
+        <v>0.36875</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>2</v>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9">
-        <v>5.375</v>
+        <v>6.25</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9">
         <v>1.3125</v>
       </c>
       <c r="H9">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J9">
-        <v>0.28125</v>
+        <v>0.4562499999999999</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>2</v>
+      <c r="B10" t="s">
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>0.475</v>
+        <v>0.675</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
       <c r="E10">
-        <v>3.40625</v>
+        <v>6.6875</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G10">
-        <v>1.40625</v>
+        <v>1.21875</v>
       </c>
       <c r="H10">
         <v>67.5</v>
@@ -733,36 +739,36 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <v>0.478125</v>
+        <v>0.303125</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>2</v>
+      <c r="B11" t="s">
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>0.7000000000000001</v>
+        <v>0.6375000000000001</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E11">
-        <v>4.9375</v>
+        <v>1.4375</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G11">
-        <v>1.21875</v>
+        <v>0.75</v>
       </c>
       <c r="H11">
-        <v>112.5</v>
+        <v>123.75</v>
       </c>
       <c r="I11">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J11">
         <v>0.390625</v>
@@ -772,29 +778,29 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>2</v>
+      <c r="B12" t="s">
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>0.625</v>
+        <v>0.5750000000000001</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E12">
-        <v>5.8125</v>
+        <v>3.40625</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G12">
-        <v>0.46875</v>
+        <v>1.171875</v>
       </c>
       <c r="H12">
-        <v>337.5</v>
+        <v>157.5</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J12">
         <v>0.215625</v>
@@ -804,157 +810,157 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>2</v>
+      <c r="B13" t="s">
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>0.425</v>
+        <v>0.4375</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13">
-        <v>6.6875</v>
+        <v>7.125</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G13">
-        <v>0.09375</v>
+        <v>0.28125</v>
       </c>
       <c r="H13">
-        <v>292.5</v>
+        <v>202.5</v>
       </c>
       <c r="I13">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J13">
-        <v>0.434375</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>2</v>
+      <c r="B14" t="s">
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>0.6000000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E14">
-        <v>4.0625</v>
+        <v>6.90625</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>0.9375</v>
       </c>
       <c r="H14">
-        <v>157.5</v>
+        <v>22.5</v>
       </c>
       <c r="I14">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J14">
-        <v>0.3578125</v>
+        <v>0.259375</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>0.775</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>4.0625</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15">
+        <v>1.125</v>
+      </c>
+      <c r="H15">
+        <v>292.5</v>
+      </c>
+      <c r="I15">
         <v>2</v>
       </c>
-      <c r="C15">
-        <v>0.4375</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15">
-        <v>1.4375</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15">
-        <v>0.796875</v>
-      </c>
-      <c r="H15">
-        <v>22.5</v>
-      </c>
-      <c r="I15">
-        <v>23</v>
-      </c>
       <c r="J15">
-        <v>0.2703125</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>2</v>
+      <c r="B16" t="s">
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>0.775</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16">
-        <v>2.3125</v>
+        <v>4.9375</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G16">
-        <v>0.1875</v>
+        <v>0.421875</v>
       </c>
       <c r="H16">
-        <v>202.5</v>
+        <v>337.5</v>
       </c>
       <c r="I16">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J16">
-        <v>0.171875</v>
+        <v>0.19375</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>2</v>
+      <c r="B17" t="s">
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>0.6375000000000001</v>
+        <v>0.525</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>1.875</v>
+        <v>5.8125</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G17">
-        <v>0.75</v>
+        <v>1.40625</v>
       </c>
       <c r="H17">
         <v>303.75</v>
       </c>
       <c r="I17">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="J17">
         <v>0.4453125</v>
@@ -964,360 +970,360 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>2</v>
+      <c r="B18" t="s">
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>0.525</v>
+        <v>0.625</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18">
-        <v>3.625</v>
+        <v>1.65625</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G18">
-        <v>0.421875</v>
+        <v>0.09375</v>
       </c>
       <c r="H18">
-        <v>123.75</v>
+        <v>112.5</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J18">
-        <v>0.346875</v>
+        <v>0.2703125</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>2</v>
+      <c r="B19" t="s">
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>0.45</v>
+        <v>0.7375</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E19">
-        <v>1.65625</v>
+        <v>7.5625</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G19">
-        <v>0.28125</v>
+        <v>0.796875</v>
       </c>
       <c r="H19">
         <v>33.75</v>
       </c>
       <c r="I19">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J19">
-        <v>0.259375</v>
+        <v>0.3578125</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>2</v>
+      <c r="B20" t="s">
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>0.6000000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E20">
-        <v>7.125</v>
+        <v>6.25</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G20">
-        <v>1.21875</v>
+        <v>0.65625</v>
       </c>
       <c r="H20">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="I20">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J20">
-        <v>0.19375</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>2</v>
+      <c r="B21" t="s">
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>0.475</v>
+        <v>0.625</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E21">
-        <v>4.0625</v>
+        <v>3.625</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G21">
-        <v>1.125</v>
+        <v>1.171875</v>
       </c>
       <c r="H21">
-        <v>292.5</v>
+        <v>225</v>
       </c>
       <c r="I21">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J21">
-        <v>0.346875</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>2</v>
+      <c r="B22" t="s">
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>0.6375000000000001</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E22">
-        <v>7.5625</v>
+        <v>2.75</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G22">
-        <v>0.796875</v>
+        <v>1.3125</v>
       </c>
       <c r="H22">
-        <v>157.5</v>
+        <v>303.75</v>
       </c>
       <c r="I22">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J22">
-        <v>0.325</v>
+        <v>0.19375</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>2</v>
+      <c r="B23" t="s">
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <v>2.3125</v>
+        <v>5.375</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G23">
-        <v>0.375</v>
+        <v>1.21875</v>
       </c>
       <c r="H23">
-        <v>270</v>
+        <v>22.5</v>
       </c>
       <c r="I23">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J23">
-        <v>0.303125</v>
+        <v>0.2375</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>2</v>
+      <c r="B24" t="s">
+        <v>9</v>
       </c>
       <c r="C24">
-        <v>0.5750000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24">
-        <v>1.875</v>
+        <v>7.125</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G24">
-        <v>1.3125</v>
+        <v>0.84375</v>
       </c>
       <c r="H24">
         <v>135</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J24">
-        <v>0.4453125</v>
+        <v>0.478125</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>2</v>
+      <c r="B25" t="s">
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>0.75</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E25">
         <v>3.1875</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G25">
-        <v>0.9375</v>
+        <v>1.03125</v>
       </c>
       <c r="H25">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="I25">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="J25">
-        <v>0.478125</v>
+        <v>0.36875</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>2</v>
+      <c r="B26" t="s">
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>0.675</v>
+        <v>0.45</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E26">
-        <v>3.625</v>
+        <v>1.875</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G26">
-        <v>0.1875</v>
+        <v>0.75</v>
       </c>
       <c r="H26">
-        <v>45</v>
+        <v>337.5</v>
       </c>
       <c r="I26">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J26">
-        <v>0.215625</v>
+        <v>0.346875</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>2</v>
+      <c r="B27" t="s">
+        <v>9</v>
       </c>
       <c r="C27">
-        <v>0.7000000000000001</v>
+        <v>0.675</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E27">
-        <v>6.25</v>
+        <v>4.5</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G27">
-        <v>0.84375</v>
+        <v>0.9375</v>
       </c>
       <c r="H27">
-        <v>247.5</v>
+        <v>45</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="J27">
-        <v>0.36875</v>
+        <v>0.215625</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>2</v>
+      <c r="B28" t="s">
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>0.45</v>
+        <v>0.475</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28">
         <v>6.6875</v>
       </c>
       <c r="F28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G28">
         <v>0.09375</v>
       </c>
       <c r="H28">
-        <v>67.5</v>
+        <v>247.5</v>
       </c>
       <c r="I28">
         <v>14</v>
       </c>
       <c r="J28">
-        <v>0.4125</v>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>2</v>
+      <c r="B29" t="s">
+        <v>9</v>
       </c>
       <c r="C29">
         <v>0.525</v>
@@ -1326,138 +1332,138 @@
         <v>11</v>
       </c>
       <c r="E29">
-        <v>4.5</v>
+        <v>6.90625</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G29">
-        <v>1.40625</v>
+        <v>0.796875</v>
       </c>
       <c r="H29">
-        <v>90</v>
+        <v>202.5</v>
       </c>
       <c r="I29">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="J29">
-        <v>0.4562499999999999</v>
+        <v>0.171875</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>2</v>
+      <c r="B30" t="s">
+        <v>9</v>
       </c>
       <c r="C30">
-        <v>0.775</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30">
-        <v>5.8125</v>
+        <v>4.0625</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G30">
-        <v>0.75</v>
+        <v>1.125</v>
       </c>
       <c r="H30">
-        <v>303.75</v>
+        <v>157.5</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J30">
-        <v>0.390625</v>
+        <v>0.259375</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>2</v>
+      <c r="B31" t="s">
+        <v>9</v>
       </c>
       <c r="C31">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31">
-        <v>6.90625</v>
+        <v>4.9375</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G31">
-        <v>0.46875</v>
+        <v>0.375</v>
       </c>
       <c r="H31">
-        <v>337.5</v>
+        <v>67.5</v>
       </c>
       <c r="I31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J31">
-        <v>0.434375</v>
+        <v>0.2703125</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>2</v>
+      <c r="B32" t="s">
+        <v>9</v>
       </c>
       <c r="C32">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E32">
-        <v>5.375</v>
+        <v>3.40625</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G32">
-        <v>1.03125</v>
+        <v>0.1875</v>
       </c>
       <c r="H32">
-        <v>315</v>
+        <v>123.75</v>
       </c>
       <c r="I32">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J32">
-        <v>0.2703125</v>
+        <v>0.4453125</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>2</v>
+      <c r="B33" t="s">
+        <v>9</v>
       </c>
       <c r="C33">
-        <v>0.4375</v>
+        <v>0.5750000000000001</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E33">
-        <v>1.4375</v>
+        <v>2.3125</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G33">
         <v>0.28125</v>
@@ -1466,129 +1472,129 @@
         <v>112.5</v>
       </c>
       <c r="I33">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="J33">
-        <v>0.2375</v>
+        <v>0.434375</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>2</v>
+      <c r="B34" t="s">
+        <v>9</v>
       </c>
       <c r="C34">
-        <v>0.7250000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E34">
-        <v>4.9375</v>
+        <v>5.8125</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G34">
-        <v>0.65625</v>
+        <v>0.5625</v>
       </c>
       <c r="H34">
-        <v>22.5</v>
+        <v>180</v>
       </c>
       <c r="I34">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J34">
-        <v>0.171875</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>2</v>
+      <c r="B35" t="s">
+        <v>9</v>
       </c>
       <c r="C35">
-        <v>0.65</v>
+        <v>0.4375</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E35">
-        <v>2.75</v>
+        <v>1.4375</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G35">
         <v>0.421875</v>
       </c>
       <c r="H35">
-        <v>123.75</v>
+        <v>292.5</v>
       </c>
       <c r="I35">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J35">
-        <v>0.259375</v>
+        <v>0.303125</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36">
-        <v>2</v>
+      <c r="B36" t="s">
+        <v>9</v>
       </c>
       <c r="C36">
-        <v>0.7375</v>
+        <v>0.6375000000000001</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E36">
-        <v>3.40625</v>
+        <v>7.5625</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G36">
-        <v>1.171875</v>
+        <v>1.40625</v>
       </c>
       <c r="H36">
-        <v>202.5</v>
+        <v>90</v>
       </c>
       <c r="I36">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J36">
-        <v>0.28125</v>
+        <v>0.4562499999999999</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>2</v>
+      <c r="B37" t="s">
+        <v>9</v>
       </c>
       <c r="C37">
-        <v>0.425</v>
+        <v>0.7375</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E37">
         <v>1.65625</v>
       </c>
       <c r="F37" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G37">
-        <v>0.5625</v>
+        <v>0.46875</v>
       </c>
       <c r="H37">
         <v>33.75</v>
@@ -1604,61 +1610,61 @@
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>2</v>
+      <c r="B38" t="s">
+        <v>9</v>
       </c>
       <c r="C38">
-        <v>0.7000000000000001</v>
+        <v>0.675</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E38">
-        <v>6.25</v>
+        <v>4.5</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G38">
-        <v>1.125</v>
+        <v>0.375</v>
       </c>
       <c r="H38">
         <v>180</v>
       </c>
       <c r="I38">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="J38">
-        <v>0.390625</v>
+        <v>0.259375</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>2</v>
+      <c r="B39" t="s">
+        <v>9</v>
       </c>
       <c r="C39">
-        <v>0.425</v>
+        <v>0.625</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E39">
-        <v>5.375</v>
+        <v>2.75</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G39">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="H39">
-        <v>157.5</v>
+        <v>225</v>
       </c>
       <c r="I39">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J39">
         <v>0.4562499999999999</v>
@@ -1668,573 +1674,573 @@
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>2</v>
+      <c r="B40" t="s">
+        <v>9</v>
       </c>
       <c r="C40">
-        <v>0.5</v>
+        <v>0.525</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E40">
-        <v>3.625</v>
+        <v>6.25</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G40">
-        <v>0.84375</v>
+        <v>0.65625</v>
       </c>
       <c r="H40">
-        <v>135</v>
+        <v>270</v>
       </c>
       <c r="I40">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="J40">
-        <v>0.325</v>
+        <v>0.2375</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41">
-        <v>2</v>
+      <c r="B41" t="s">
+        <v>9</v>
       </c>
       <c r="C41">
-        <v>0.775</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E41">
-        <v>3.1875</v>
+        <v>5.375</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G41">
-        <v>0.796875</v>
+        <v>0.46875</v>
       </c>
       <c r="H41">
-        <v>90</v>
+        <v>33.75</v>
       </c>
       <c r="I41">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="J41">
-        <v>0.4125</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42">
+        <v>0.45</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <v>7.125</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>1.3125</v>
+      </c>
+      <c r="H42">
+        <v>67.5</v>
+      </c>
+      <c r="I42">
         <v>2</v>
       </c>
-      <c r="C42">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42">
-        <v>6.90625</v>
-      </c>
-      <c r="F42" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42">
-        <v>0.1875</v>
-      </c>
-      <c r="H42">
-        <v>22.5</v>
-      </c>
-      <c r="I42">
-        <v>6</v>
-      </c>
       <c r="J42">
-        <v>0.19375</v>
+        <v>0.2703125</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43">
-        <v>2</v>
+      <c r="B43" t="s">
+        <v>9</v>
       </c>
       <c r="C43">
-        <v>0.475</v>
+        <v>0.75</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E43">
         <v>1.875</v>
       </c>
       <c r="F43" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G43">
-        <v>0.46875</v>
+        <v>0.5625</v>
       </c>
       <c r="H43">
-        <v>123.75</v>
+        <v>90</v>
       </c>
       <c r="I43">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J43">
-        <v>0.28125</v>
+        <v>0.19375</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44">
-        <v>2</v>
+      <c r="B44" t="s">
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>0.65</v>
+        <v>0.475</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E44">
-        <v>7.125</v>
+        <v>3.1875</v>
       </c>
       <c r="F44" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G44">
-        <v>1.03125</v>
+        <v>0.84375</v>
       </c>
       <c r="H44">
-        <v>202.5</v>
+        <v>45</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J44">
-        <v>0.478125</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45">
-        <v>2</v>
+      <c r="B45" t="s">
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>0.55</v>
+        <v>0.65</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E45">
-        <v>4.5</v>
+        <v>3.625</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G45">
-        <v>0.421875</v>
+        <v>0.1875</v>
       </c>
       <c r="H45">
-        <v>67.5</v>
+        <v>337.5</v>
       </c>
       <c r="I45">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J45">
-        <v>0.36875</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>2</v>
+      <c r="B46" t="s">
+        <v>9</v>
       </c>
       <c r="C46">
-        <v>0.675</v>
+        <v>0.55</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E46">
         <v>6.6875</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G46">
         <v>0.09375</v>
       </c>
       <c r="H46">
-        <v>247.5</v>
+        <v>157.5</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J46">
-        <v>0.4453125</v>
+        <v>0.303125</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47">
-        <v>2</v>
+      <c r="B47" t="s">
+        <v>9</v>
       </c>
       <c r="C47">
-        <v>0.45</v>
+        <v>0.6375000000000001</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E47">
-        <v>2.3125</v>
+        <v>7.5625</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G47">
-        <v>1.171875</v>
+        <v>1.125</v>
       </c>
       <c r="H47">
-        <v>112.5</v>
+        <v>123.75</v>
       </c>
       <c r="I47">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J47">
-        <v>0.303125</v>
+        <v>0.434375</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48">
-        <v>2</v>
+      <c r="B48" t="s">
+        <v>9</v>
       </c>
       <c r="C48">
-        <v>0.5750000000000001</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E48">
-        <v>3.40625</v>
+        <v>4.0625</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G48">
-        <v>0.28125</v>
+        <v>1.171875</v>
       </c>
       <c r="H48">
-        <v>337.5</v>
+        <v>247.5</v>
       </c>
       <c r="I48">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J48">
-        <v>0.2703125</v>
+        <v>0.346875</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49">
-        <v>2</v>
+      <c r="B49" t="s">
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>0.7250000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E49">
-        <v>4.9375</v>
+        <v>3.40625</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G49">
-        <v>1.3125</v>
+        <v>1.40625</v>
       </c>
       <c r="H49">
-        <v>303.75</v>
+        <v>112.5</v>
       </c>
       <c r="I49">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="J49">
-        <v>0.215625</v>
+        <v>0.3578125</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50">
-        <v>2</v>
+      <c r="B50" t="s">
+        <v>9</v>
       </c>
       <c r="C50">
-        <v>0.7375</v>
+        <v>0.4375</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E50">
-        <v>1.4375</v>
+        <v>4.9375</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G50">
-        <v>0.65625</v>
+        <v>0.9375</v>
       </c>
       <c r="H50">
         <v>292.5</v>
       </c>
       <c r="I50">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J50">
-        <v>0.2375</v>
+        <v>0.478125</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51">
-        <v>2</v>
+      <c r="B51" t="s">
+        <v>9</v>
       </c>
       <c r="C51">
-        <v>0.75</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51">
-        <v>2.75</v>
+        <v>1.4375</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G51">
-        <v>0.75</v>
+        <v>1.03125</v>
       </c>
       <c r="H51">
-        <v>315</v>
+        <v>303.75</v>
       </c>
       <c r="I51">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J51">
-        <v>0.259375</v>
+        <v>0.171875</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52">
-        <v>2</v>
+      <c r="B52" t="s">
+        <v>9</v>
       </c>
       <c r="C52">
-        <v>0.6375000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E52">
-        <v>5.8125</v>
+        <v>2.3125</v>
       </c>
       <c r="F52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G52">
-        <v>1.40625</v>
+        <v>1.21875</v>
       </c>
       <c r="H52">
-        <v>45</v>
+        <v>202.5</v>
       </c>
       <c r="I52">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="J52">
-        <v>0.434375</v>
+        <v>0.4453125</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53">
-        <v>2</v>
+      <c r="B53" t="s">
+        <v>9</v>
       </c>
       <c r="C53">
-        <v>0.625</v>
+        <v>0.5750000000000001</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E53">
-        <v>1.65625</v>
+        <v>5.8125</v>
       </c>
       <c r="F53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G53">
-        <v>1.21875</v>
+        <v>0.28125</v>
       </c>
       <c r="H53">
-        <v>225</v>
+        <v>22.5</v>
       </c>
       <c r="I53">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J53">
-        <v>0.346875</v>
+        <v>0.36875</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54">
-        <v>2</v>
+      <c r="B54" t="s">
+        <v>9</v>
       </c>
       <c r="C54">
-        <v>0.4375</v>
+        <v>0.775</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E54">
-        <v>4.0625</v>
+        <v>6.90625</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G54">
-        <v>0.9375</v>
+        <v>0.421875</v>
       </c>
       <c r="H54">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="I54">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J54">
-        <v>0.171875</v>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55">
-        <v>2</v>
+      <c r="B55" t="s">
+        <v>9</v>
       </c>
       <c r="C55">
-        <v>0.525</v>
+        <v>0.7375</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55">
-        <v>7.5625</v>
+        <v>1.65625</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G55">
-        <v>0.5625</v>
+        <v>0.796875</v>
       </c>
       <c r="H55">
-        <v>33.75</v>
+        <v>315</v>
       </c>
       <c r="I55">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J55">
-        <v>0.3578125</v>
+        <v>0.215625</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56">
-        <v>3</v>
+      <c r="B56" t="s">
+        <v>10</v>
       </c>
       <c r="C56">
-        <v>0.7250000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E56">
-        <v>6.25</v>
+        <v>4.5</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G56">
-        <v>1.125</v>
+        <v>0.5625</v>
       </c>
       <c r="H56">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="I56">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J56">
-        <v>0.4562499999999999</v>
+        <v>0.2375</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57">
-        <v>3</v>
+      <c r="B57" t="s">
+        <v>10</v>
       </c>
       <c r="C57">
-        <v>0.75</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E57">
-        <v>4.5</v>
+        <v>1.875</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G57">
-        <v>1.171875</v>
+        <v>0.65625</v>
       </c>
       <c r="H57">
-        <v>135</v>
+        <v>315</v>
       </c>
       <c r="I57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J57">
         <v>0.325</v>
@@ -2244,215 +2250,215 @@
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58">
-        <v>3</v>
+      <c r="B58" t="s">
+        <v>10</v>
       </c>
       <c r="C58">
-        <v>0.55</v>
+        <v>0.75</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E58">
-        <v>2.75</v>
+        <v>3.625</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G58">
         <v>0.84375</v>
       </c>
       <c r="H58">
-        <v>247.5</v>
+        <v>90</v>
       </c>
       <c r="I58">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J58">
-        <v>0.19375</v>
+        <v>0.346875</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59">
-        <v>3</v>
+      <c r="B59" t="s">
+        <v>10</v>
       </c>
       <c r="C59">
-        <v>0.65</v>
+        <v>0.475</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E59">
-        <v>7.5625</v>
+        <v>2.75</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G59">
-        <v>0.375</v>
+        <v>1.03125</v>
       </c>
       <c r="H59">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="I59">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J59">
-        <v>0.4125</v>
+        <v>0.171875</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60">
-        <v>3</v>
+      <c r="B60" t="s">
+        <v>10</v>
       </c>
       <c r="C60">
-        <v>0.5750000000000001</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E60">
-        <v>7.125</v>
+        <v>5.375</v>
       </c>
       <c r="F60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G60">
-        <v>0.5625</v>
+        <v>0.46875</v>
       </c>
       <c r="H60">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="I60">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J60">
-        <v>0.2375</v>
+        <v>0.434375</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61">
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>0.5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61">
+        <v>2.3125</v>
+      </c>
+      <c r="F61" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61">
+        <v>0.1875</v>
+      </c>
+      <c r="H61">
+        <v>45</v>
+      </c>
+      <c r="I61">
         <v>3</v>
       </c>
-      <c r="C61">
-        <v>0.7375</v>
-      </c>
-      <c r="D61" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61">
-        <v>6.90625</v>
-      </c>
-      <c r="F61" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61">
-        <v>0.65625</v>
-      </c>
-      <c r="H61">
-        <v>180</v>
-      </c>
-      <c r="I61">
-        <v>12</v>
-      </c>
       <c r="J61">
-        <v>0.36875</v>
+        <v>0.478125</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62">
-        <v>3</v>
+      <c r="B62" t="s">
+        <v>10</v>
       </c>
       <c r="C62">
-        <v>0.675</v>
+        <v>0.55</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E62">
         <v>3.1875</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G62">
-        <v>1.03125</v>
+        <v>0.375</v>
       </c>
       <c r="H62">
-        <v>90</v>
+        <v>247.5</v>
       </c>
       <c r="I62">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J62">
-        <v>0.303125</v>
+        <v>0.36875</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63">
-        <v>3</v>
+      <c r="B63" t="s">
+        <v>10</v>
       </c>
       <c r="C63">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E63">
-        <v>5.375</v>
+        <v>6.25</v>
       </c>
       <c r="F63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G63">
         <v>1.3125</v>
       </c>
       <c r="H63">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="I63">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J63">
-        <v>0.28125</v>
+        <v>0.4562499999999999</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64">
-        <v>3</v>
+      <c r="B64" t="s">
+        <v>10</v>
       </c>
       <c r="C64">
-        <v>0.475</v>
+        <v>0.675</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
       </c>
       <c r="E64">
-        <v>3.40625</v>
+        <v>6.6875</v>
       </c>
       <c r="F64" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G64">
-        <v>1.40625</v>
+        <v>1.21875</v>
       </c>
       <c r="H64">
         <v>67.5</v>
@@ -2461,36 +2467,36 @@
         <v>14</v>
       </c>
       <c r="J64">
-        <v>0.478125</v>
+        <v>0.303125</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65">
-        <v>3</v>
+      <c r="B65" t="s">
+        <v>10</v>
       </c>
       <c r="C65">
-        <v>0.7000000000000001</v>
+        <v>0.6375000000000001</v>
       </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E65">
-        <v>4.9375</v>
+        <v>1.4375</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G65">
-        <v>1.21875</v>
+        <v>0.75</v>
       </c>
       <c r="H65">
-        <v>112.5</v>
+        <v>123.75</v>
       </c>
       <c r="I65">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J65">
         <v>0.390625</v>
@@ -2500,29 +2506,29 @@
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66">
-        <v>3</v>
+      <c r="B66" t="s">
+        <v>10</v>
       </c>
       <c r="C66">
-        <v>0.625</v>
+        <v>0.5750000000000001</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E66">
-        <v>5.8125</v>
+        <v>3.40625</v>
       </c>
       <c r="F66" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G66">
-        <v>0.46875</v>
+        <v>1.171875</v>
       </c>
       <c r="H66">
-        <v>337.5</v>
+        <v>157.5</v>
       </c>
       <c r="I66">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J66">
         <v>0.215625</v>
@@ -2532,157 +2538,157 @@
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67">
-        <v>3</v>
+      <c r="B67" t="s">
+        <v>10</v>
       </c>
       <c r="C67">
-        <v>0.425</v>
+        <v>0.4375</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E67">
-        <v>6.6875</v>
+        <v>7.125</v>
       </c>
       <c r="F67" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G67">
-        <v>0.09375</v>
+        <v>0.28125</v>
       </c>
       <c r="H67">
-        <v>292.5</v>
+        <v>202.5</v>
       </c>
       <c r="I67">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J67">
-        <v>0.434375</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68">
-        <v>3</v>
+      <c r="B68" t="s">
+        <v>10</v>
       </c>
       <c r="C68">
-        <v>0.6000000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E68">
-        <v>4.0625</v>
+        <v>6.90625</v>
       </c>
       <c r="F68" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G68">
         <v>0.9375</v>
       </c>
       <c r="H68">
-        <v>157.5</v>
+        <v>22.5</v>
       </c>
       <c r="I68">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J68">
-        <v>0.3578125</v>
+        <v>0.259375</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69">
-        <v>3</v>
+      <c r="B69" t="s">
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>0.4375</v>
+        <v>0.775</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E69">
-        <v>1.4375</v>
+        <v>4.0625</v>
       </c>
       <c r="F69" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G69">
-        <v>0.796875</v>
+        <v>1.125</v>
       </c>
       <c r="H69">
-        <v>22.5</v>
+        <v>292.5</v>
       </c>
       <c r="I69">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="J69">
-        <v>0.2703125</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70">
-        <v>3</v>
+      <c r="B70" t="s">
+        <v>10</v>
       </c>
       <c r="C70">
-        <v>0.775</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E70">
-        <v>2.3125</v>
+        <v>4.9375</v>
       </c>
       <c r="F70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G70">
-        <v>0.1875</v>
+        <v>0.421875</v>
       </c>
       <c r="H70">
-        <v>202.5</v>
+        <v>337.5</v>
       </c>
       <c r="I70">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="J70">
-        <v>0.171875</v>
+        <v>0.19375</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71">
-        <v>3</v>
+      <c r="B71" t="s">
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>0.6375000000000001</v>
+        <v>0.525</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E71">
-        <v>1.875</v>
+        <v>5.8125</v>
       </c>
       <c r="F71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G71">
-        <v>0.75</v>
+        <v>1.40625</v>
       </c>
       <c r="H71">
         <v>303.75</v>
       </c>
       <c r="I71">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="J71">
         <v>0.4453125</v>
@@ -2692,360 +2698,360 @@
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72">
-        <v>3</v>
+      <c r="B72" t="s">
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>0.525</v>
+        <v>0.625</v>
       </c>
       <c r="D72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E72">
-        <v>3.625</v>
+        <v>1.65625</v>
       </c>
       <c r="F72" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G72">
-        <v>0.421875</v>
+        <v>0.09375</v>
       </c>
       <c r="H72">
-        <v>123.75</v>
+        <v>112.5</v>
       </c>
       <c r="I72">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J72">
-        <v>0.346875</v>
+        <v>0.2703125</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>71</v>
       </c>
-      <c r="B73">
-        <v>3</v>
+      <c r="B73" t="s">
+        <v>10</v>
       </c>
       <c r="C73">
-        <v>0.45</v>
+        <v>0.7375</v>
       </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E73">
-        <v>1.65625</v>
+        <v>7.5625</v>
       </c>
       <c r="F73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G73">
-        <v>0.28125</v>
+        <v>0.796875</v>
       </c>
       <c r="H73">
         <v>33.75</v>
       </c>
       <c r="I73">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J73">
-        <v>0.259375</v>
+        <v>0.3578125</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74">
-        <v>3</v>
+      <c r="B74" t="s">
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>0.6000000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E74">
-        <v>7.125</v>
+        <v>6.25</v>
       </c>
       <c r="F74" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G74">
-        <v>1.21875</v>
+        <v>0.65625</v>
       </c>
       <c r="H74">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="I74">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J74">
-        <v>0.19375</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75">
-        <v>3</v>
+      <c r="B75" t="s">
+        <v>10</v>
       </c>
       <c r="C75">
-        <v>0.475</v>
+        <v>0.625</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E75">
-        <v>4.0625</v>
+        <v>3.625</v>
       </c>
       <c r="F75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G75">
-        <v>1.125</v>
+        <v>1.171875</v>
       </c>
       <c r="H75">
-        <v>292.5</v>
+        <v>225</v>
       </c>
       <c r="I75">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J75">
-        <v>0.346875</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B76">
-        <v>3</v>
+      <c r="B76" t="s">
+        <v>10</v>
       </c>
       <c r="C76">
-        <v>0.6375000000000001</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E76">
-        <v>7.5625</v>
+        <v>2.75</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G76">
-        <v>0.796875</v>
+        <v>1.3125</v>
       </c>
       <c r="H76">
-        <v>157.5</v>
+        <v>303.75</v>
       </c>
       <c r="I76">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J76">
-        <v>0.325</v>
+        <v>0.19375</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B77">
-        <v>3</v>
+      <c r="B77" t="s">
+        <v>10</v>
       </c>
       <c r="C77">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E77">
-        <v>2.3125</v>
+        <v>5.375</v>
       </c>
       <c r="F77" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G77">
-        <v>0.375</v>
+        <v>1.21875</v>
       </c>
       <c r="H77">
-        <v>270</v>
+        <v>22.5</v>
       </c>
       <c r="I77">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J77">
-        <v>0.303125</v>
+        <v>0.2375</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78">
-        <v>3</v>
+      <c r="B78" t="s">
+        <v>10</v>
       </c>
       <c r="C78">
-        <v>0.5750000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E78">
-        <v>1.875</v>
+        <v>7.125</v>
       </c>
       <c r="F78" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G78">
-        <v>1.3125</v>
+        <v>0.84375</v>
       </c>
       <c r="H78">
         <v>135</v>
       </c>
       <c r="I78">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J78">
-        <v>0.4453125</v>
+        <v>0.478125</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79">
-        <v>3</v>
+      <c r="B79" t="s">
+        <v>10</v>
       </c>
       <c r="C79">
-        <v>0.75</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E79">
         <v>3.1875</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G79">
-        <v>0.9375</v>
+        <v>1.03125</v>
       </c>
       <c r="H79">
-        <v>225</v>
+        <v>315</v>
       </c>
       <c r="I79">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="J79">
-        <v>0.478125</v>
+        <v>0.36875</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80">
-        <v>3</v>
+      <c r="B80" t="s">
+        <v>10</v>
       </c>
       <c r="C80">
-        <v>0.675</v>
+        <v>0.45</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E80">
-        <v>3.625</v>
+        <v>1.875</v>
       </c>
       <c r="F80" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G80">
-        <v>0.1875</v>
+        <v>0.75</v>
       </c>
       <c r="H80">
-        <v>45</v>
+        <v>337.5</v>
       </c>
       <c r="I80">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J80">
-        <v>0.215625</v>
+        <v>0.346875</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81">
-        <v>3</v>
+      <c r="B81" t="s">
+        <v>10</v>
       </c>
       <c r="C81">
-        <v>0.7000000000000001</v>
+        <v>0.675</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E81">
-        <v>6.25</v>
+        <v>4.5</v>
       </c>
       <c r="F81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G81">
-        <v>0.84375</v>
+        <v>0.9375</v>
       </c>
       <c r="H81">
-        <v>247.5</v>
+        <v>45</v>
       </c>
       <c r="I81">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="J81">
-        <v>0.36875</v>
+        <v>0.215625</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82">
-        <v>3</v>
+      <c r="B82" t="s">
+        <v>10</v>
       </c>
       <c r="C82">
-        <v>0.45</v>
+        <v>0.475</v>
       </c>
       <c r="D82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E82">
         <v>6.6875</v>
       </c>
       <c r="F82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G82">
         <v>0.09375</v>
       </c>
       <c r="H82">
-        <v>67.5</v>
+        <v>247.5</v>
       </c>
       <c r="I82">
         <v>14</v>
       </c>
       <c r="J82">
-        <v>0.4125</v>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83">
-        <v>3</v>
+      <c r="B83" t="s">
+        <v>10</v>
       </c>
       <c r="C83">
         <v>0.525</v>
@@ -3054,138 +3060,138 @@
         <v>11</v>
       </c>
       <c r="E83">
-        <v>4.5</v>
+        <v>6.90625</v>
       </c>
       <c r="F83" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G83">
-        <v>1.40625</v>
+        <v>0.796875</v>
       </c>
       <c r="H83">
-        <v>90</v>
+        <v>202.5</v>
       </c>
       <c r="I83">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="J83">
-        <v>0.4562499999999999</v>
+        <v>0.171875</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84">
-        <v>3</v>
+      <c r="B84" t="s">
+        <v>10</v>
       </c>
       <c r="C84">
-        <v>0.775</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
       </c>
       <c r="E84">
-        <v>5.8125</v>
+        <v>4.0625</v>
       </c>
       <c r="F84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G84">
-        <v>0.75</v>
+        <v>1.125</v>
       </c>
       <c r="H84">
-        <v>303.75</v>
+        <v>157.5</v>
       </c>
       <c r="I84">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J84">
-        <v>0.390625</v>
+        <v>0.259375</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85">
-        <v>3</v>
+      <c r="B85" t="s">
+        <v>10</v>
       </c>
       <c r="C85">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
       </c>
       <c r="E85">
-        <v>6.90625</v>
+        <v>4.9375</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G85">
-        <v>0.46875</v>
+        <v>0.375</v>
       </c>
       <c r="H85">
-        <v>337.5</v>
+        <v>67.5</v>
       </c>
       <c r="I85">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J85">
-        <v>0.434375</v>
+        <v>0.2703125</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>84</v>
       </c>
-      <c r="B86">
-        <v>3</v>
+      <c r="B86" t="s">
+        <v>10</v>
       </c>
       <c r="C86">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E86">
-        <v>5.375</v>
+        <v>3.40625</v>
       </c>
       <c r="F86" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G86">
-        <v>1.03125</v>
+        <v>0.1875</v>
       </c>
       <c r="H86">
-        <v>315</v>
+        <v>123.75</v>
       </c>
       <c r="I86">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J86">
-        <v>0.2703125</v>
+        <v>0.4453125</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87">
-        <v>3</v>
+      <c r="B87" t="s">
+        <v>10</v>
       </c>
       <c r="C87">
-        <v>0.4375</v>
+        <v>0.5750000000000001</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E87">
-        <v>1.4375</v>
+        <v>2.3125</v>
       </c>
       <c r="F87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G87">
         <v>0.28125</v>
@@ -3194,129 +3200,129 @@
         <v>112.5</v>
       </c>
       <c r="I87">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="J87">
-        <v>0.2375</v>
+        <v>0.434375</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88">
-        <v>3</v>
+      <c r="B88" t="s">
+        <v>10</v>
       </c>
       <c r="C88">
-        <v>0.7250000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="D88" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E88">
-        <v>4.9375</v>
+        <v>5.8125</v>
       </c>
       <c r="F88" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G88">
-        <v>0.65625</v>
+        <v>0.5625</v>
       </c>
       <c r="H88">
-        <v>22.5</v>
+        <v>180</v>
       </c>
       <c r="I88">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J88">
-        <v>0.171875</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89">
-        <v>3</v>
+      <c r="B89" t="s">
+        <v>10</v>
       </c>
       <c r="C89">
-        <v>0.65</v>
+        <v>0.4375</v>
       </c>
       <c r="D89" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E89">
-        <v>2.75</v>
+        <v>1.4375</v>
       </c>
       <c r="F89" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G89">
         <v>0.421875</v>
       </c>
       <c r="H89">
-        <v>123.75</v>
+        <v>292.5</v>
       </c>
       <c r="I89">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J89">
-        <v>0.259375</v>
+        <v>0.303125</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90">
-        <v>3</v>
+      <c r="B90" t="s">
+        <v>10</v>
       </c>
       <c r="C90">
-        <v>0.7375</v>
+        <v>0.6375000000000001</v>
       </c>
       <c r="D90" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E90">
-        <v>3.40625</v>
+        <v>7.5625</v>
       </c>
       <c r="F90" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G90">
-        <v>1.171875</v>
+        <v>1.40625</v>
       </c>
       <c r="H90">
-        <v>202.5</v>
+        <v>90</v>
       </c>
       <c r="I90">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J90">
-        <v>0.28125</v>
+        <v>0.4562499999999999</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91">
-        <v>3</v>
+      <c r="B91" t="s">
+        <v>10</v>
       </c>
       <c r="C91">
-        <v>0.425</v>
+        <v>0.7375</v>
       </c>
       <c r="D91" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E91">
         <v>1.65625</v>
       </c>
       <c r="F91" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G91">
-        <v>0.5625</v>
+        <v>0.46875</v>
       </c>
       <c r="H91">
         <v>33.75</v>
@@ -3332,61 +3338,61 @@
       <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92">
-        <v>3</v>
+      <c r="B92" t="s">
+        <v>10</v>
       </c>
       <c r="C92">
-        <v>0.7000000000000001</v>
+        <v>0.675</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E92">
-        <v>6.25</v>
+        <v>4.5</v>
       </c>
       <c r="F92" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G92">
-        <v>1.125</v>
+        <v>0.375</v>
       </c>
       <c r="H92">
         <v>180</v>
       </c>
       <c r="I92">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="J92">
-        <v>0.390625</v>
+        <v>0.259375</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93">
-        <v>3</v>
+      <c r="B93" t="s">
+        <v>10</v>
       </c>
       <c r="C93">
-        <v>0.425</v>
+        <v>0.625</v>
       </c>
       <c r="D93" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E93">
-        <v>5.375</v>
+        <v>2.75</v>
       </c>
       <c r="F93" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G93">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="H93">
-        <v>157.5</v>
+        <v>225</v>
       </c>
       <c r="I93">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J93">
         <v>0.4562499999999999</v>
@@ -3396,512 +3402,512 @@
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94">
+      <c r="B94" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94">
+        <v>0.525</v>
+      </c>
+      <c r="D94" t="s">
+        <v>13</v>
+      </c>
+      <c r="E94">
+        <v>6.25</v>
+      </c>
+      <c r="F94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94">
+        <v>0.65625</v>
+      </c>
+      <c r="H94">
+        <v>270</v>
+      </c>
+      <c r="I94">
         <v>3</v>
       </c>
-      <c r="C94">
-        <v>0.5</v>
-      </c>
-      <c r="D94" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94">
-        <v>3.625</v>
-      </c>
-      <c r="F94" t="s">
-        <v>13</v>
-      </c>
-      <c r="G94">
-        <v>0.84375</v>
-      </c>
-      <c r="H94">
-        <v>135</v>
-      </c>
-      <c r="I94">
-        <v>13</v>
-      </c>
       <c r="J94">
-        <v>0.325</v>
+        <v>0.2375</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95">
-        <v>3</v>
+      <c r="B95" t="s">
+        <v>10</v>
       </c>
       <c r="C95">
-        <v>0.775</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="D95" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E95">
-        <v>3.1875</v>
+        <v>5.375</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G95">
-        <v>0.796875</v>
+        <v>0.46875</v>
       </c>
       <c r="H95">
-        <v>90</v>
+        <v>33.75</v>
       </c>
       <c r="I95">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="J95">
-        <v>0.4125</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96">
-        <v>3</v>
+      <c r="B96" t="s">
+        <v>10</v>
       </c>
       <c r="C96">
-        <v>0.6000000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="D96" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E96">
-        <v>6.90625</v>
+        <v>7.125</v>
       </c>
       <c r="F96" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G96">
-        <v>0.1875</v>
+        <v>1.3125</v>
       </c>
       <c r="H96">
-        <v>22.5</v>
+        <v>67.5</v>
       </c>
       <c r="I96">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J96">
-        <v>0.19375</v>
+        <v>0.2703125</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>95</v>
       </c>
-      <c r="B97">
-        <v>3</v>
+      <c r="B97" t="s">
+        <v>10</v>
       </c>
       <c r="C97">
-        <v>0.475</v>
+        <v>0.75</v>
       </c>
       <c r="D97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E97">
         <v>1.875</v>
       </c>
       <c r="F97" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G97">
-        <v>0.46875</v>
+        <v>0.5625</v>
       </c>
       <c r="H97">
-        <v>123.75</v>
+        <v>90</v>
       </c>
       <c r="I97">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J97">
-        <v>0.28125</v>
+        <v>0.19375</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98">
-        <v>3</v>
+      <c r="B98" t="s">
+        <v>10</v>
       </c>
       <c r="C98">
-        <v>0.65</v>
+        <v>0.475</v>
       </c>
       <c r="D98" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E98">
-        <v>7.125</v>
+        <v>3.1875</v>
       </c>
       <c r="F98" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G98">
-        <v>1.03125</v>
+        <v>0.84375</v>
       </c>
       <c r="H98">
-        <v>202.5</v>
+        <v>45</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J98">
-        <v>0.478125</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99">
-        <v>3</v>
+      <c r="B99" t="s">
+        <v>10</v>
       </c>
       <c r="C99">
-        <v>0.55</v>
+        <v>0.65</v>
       </c>
       <c r="D99" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E99">
-        <v>4.5</v>
+        <v>3.625</v>
       </c>
       <c r="F99" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G99">
-        <v>0.421875</v>
+        <v>0.1875</v>
       </c>
       <c r="H99">
-        <v>67.5</v>
+        <v>337.5</v>
       </c>
       <c r="I99">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="J99">
-        <v>0.36875</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100">
-        <v>3</v>
+      <c r="B100" t="s">
+        <v>10</v>
       </c>
       <c r="C100">
-        <v>0.675</v>
+        <v>0.55</v>
       </c>
       <c r="D100" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E100">
         <v>6.6875</v>
       </c>
       <c r="F100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G100">
         <v>0.09375</v>
       </c>
       <c r="H100">
-        <v>247.5</v>
+        <v>157.5</v>
       </c>
       <c r="I100">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J100">
-        <v>0.4453125</v>
+        <v>0.303125</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101">
-        <v>3</v>
+      <c r="B101" t="s">
+        <v>10</v>
       </c>
       <c r="C101">
-        <v>0.45</v>
+        <v>0.6375000000000001</v>
       </c>
       <c r="D101" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E101">
-        <v>2.3125</v>
+        <v>7.5625</v>
       </c>
       <c r="F101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G101">
-        <v>1.171875</v>
+        <v>1.125</v>
       </c>
       <c r="H101">
-        <v>112.5</v>
+        <v>123.75</v>
       </c>
       <c r="I101">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J101">
-        <v>0.303125</v>
+        <v>0.434375</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102">
-        <v>3</v>
+      <c r="B102" t="s">
+        <v>10</v>
       </c>
       <c r="C102">
-        <v>0.5750000000000001</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="D102" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E102">
-        <v>3.40625</v>
+        <v>4.0625</v>
       </c>
       <c r="F102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G102">
-        <v>0.28125</v>
+        <v>1.171875</v>
       </c>
       <c r="H102">
-        <v>337.5</v>
+        <v>247.5</v>
       </c>
       <c r="I102">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J102">
-        <v>0.2703125</v>
+        <v>0.346875</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>101</v>
       </c>
-      <c r="B103">
-        <v>3</v>
+      <c r="B103" t="s">
+        <v>10</v>
       </c>
       <c r="C103">
-        <v>0.7250000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="D103" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E103">
-        <v>4.9375</v>
+        <v>3.40625</v>
       </c>
       <c r="F103" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G103">
-        <v>1.3125</v>
+        <v>1.40625</v>
       </c>
       <c r="H103">
-        <v>303.75</v>
+        <v>112.5</v>
       </c>
       <c r="I103">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="J103">
-        <v>0.215625</v>
+        <v>0.3578125</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104">
-        <v>3</v>
+      <c r="B104" t="s">
+        <v>10</v>
       </c>
       <c r="C104">
-        <v>0.7375</v>
+        <v>0.4375</v>
       </c>
       <c r="D104" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E104">
-        <v>1.4375</v>
+        <v>4.9375</v>
       </c>
       <c r="F104" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G104">
-        <v>0.65625</v>
+        <v>0.9375</v>
       </c>
       <c r="H104">
         <v>292.5</v>
       </c>
       <c r="I104">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J104">
-        <v>0.2375</v>
+        <v>0.478125</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105">
-        <v>3</v>
+      <c r="B105" t="s">
+        <v>10</v>
       </c>
       <c r="C105">
-        <v>0.75</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="D105" t="s">
         <v>11</v>
       </c>
       <c r="E105">
-        <v>2.75</v>
+        <v>1.4375</v>
       </c>
       <c r="F105" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G105">
-        <v>0.75</v>
+        <v>1.03125</v>
       </c>
       <c r="H105">
-        <v>315</v>
+        <v>303.75</v>
       </c>
       <c r="I105">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J105">
-        <v>0.259375</v>
+        <v>0.171875</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106">
-        <v>3</v>
+      <c r="B106" t="s">
+        <v>10</v>
       </c>
       <c r="C106">
-        <v>0.6375000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="D106" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E106">
-        <v>5.8125</v>
+        <v>2.3125</v>
       </c>
       <c r="F106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G106">
-        <v>1.40625</v>
+        <v>1.21875</v>
       </c>
       <c r="H106">
-        <v>45</v>
+        <v>202.5</v>
       </c>
       <c r="I106">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="J106">
-        <v>0.434375</v>
+        <v>0.4453125</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107">
-        <v>3</v>
+      <c r="B107" t="s">
+        <v>10</v>
       </c>
       <c r="C107">
-        <v>0.625</v>
+        <v>0.5750000000000001</v>
       </c>
       <c r="D107" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E107">
-        <v>1.65625</v>
+        <v>5.8125</v>
       </c>
       <c r="F107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G107">
-        <v>1.21875</v>
+        <v>0.28125</v>
       </c>
       <c r="H107">
-        <v>225</v>
+        <v>22.5</v>
       </c>
       <c r="I107">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J107">
-        <v>0.346875</v>
+        <v>0.36875</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>106</v>
       </c>
-      <c r="B108">
-        <v>3</v>
+      <c r="B108" t="s">
+        <v>10</v>
       </c>
       <c r="C108">
-        <v>0.4375</v>
+        <v>0.775</v>
       </c>
       <c r="D108" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E108">
-        <v>4.0625</v>
+        <v>6.90625</v>
       </c>
       <c r="F108" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G108">
-        <v>0.9375</v>
+        <v>0.421875</v>
       </c>
       <c r="H108">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="I108">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J108">
-        <v>0.171875</v>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109">
-        <v>3</v>
+      <c r="B109" t="s">
+        <v>10</v>
       </c>
       <c r="C109">
-        <v>0.525</v>
+        <v>0.7375</v>
       </c>
       <c r="D109" t="s">
         <v>11</v>
       </c>
       <c r="E109">
-        <v>7.5625</v>
+        <v>1.65625</v>
       </c>
       <c r="F109" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G109">
-        <v>0.5625</v>
+        <v>0.796875</v>
       </c>
       <c r="H109">
-        <v>33.75</v>
+        <v>315</v>
       </c>
       <c r="I109">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J109">
-        <v>0.3578125</v>
+        <v>0.215625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>